<commit_message>
mobile home page update
</commit_message>
<xml_diff>
--- a/code_managment.xlsx
+++ b/code_managment.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="20955" windowHeight="9975"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="20955" windowHeight="9975" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Website" sheetId="1" r:id="rId1"/>
     <sheet name="Mobile" sheetId="4" r:id="rId2"/>
     <sheet name="Admin" sheetId="5" r:id="rId3"/>
     <sheet name="Server" sheetId="6" r:id="rId4"/>
+    <sheet name="Testing - Revisions" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Admin!$A$1:$D$2</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
   <si>
     <t>location</t>
   </si>
@@ -218,6 +219,21 @@
   </si>
   <si>
     <t>re-instate only revision in last revision</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>view home page with login link</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t>Add/delete section</t>
+  </si>
+  <si>
+    <t>Add/delete clause</t>
   </si>
 </sst>
 </file>
@@ -568,8 +584,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,10 +899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,6 +960,17 @@
       </c>
       <c r="D6" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1089,4 +1116,37 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="B7:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Product functionality incorporation ph1
addition of models and controllers for product data functionality
general corrections to rendering of line text
</commit_message>
<xml_diff>
--- a/code_managment.xlsx
+++ b/code_managment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="20955" windowHeight="9975" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="20955" windowHeight="9975"/>
   </bookViews>
   <sheets>
     <sheet name="Website" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Admin!$A$1:$D$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Mobile!$A$1:$D$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Server!$A$1:$D$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Website!$A$1:$D$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Website!$A$1:$D$32</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
   <si>
     <t>location</t>
   </si>
@@ -83,9 +83,6 @@
     <t>create account</t>
   </si>
   <si>
-    <t>error on pasword does not fit in column</t>
-  </si>
-  <si>
     <t>project edit</t>
   </si>
   <si>
@@ -122,9 +119,6 @@
     <t>does logo save when company created</t>
   </si>
   <si>
-    <t>user details</t>
-  </si>
-  <si>
     <t>when linetype is change to prefix and line before has been changed the same does not work</t>
   </si>
   <si>
@@ -140,9 +134,6 @@
     <t>quote on website</t>
   </si>
   <si>
-    <t>warn that user will be automatically signed out on update</t>
-  </si>
-  <si>
     <t>add ability to create custome clause</t>
   </si>
   <si>
@@ -173,9 +164,6 @@
     <t>delete image from project and company</t>
   </si>
   <si>
-    <t>project edit and neew errors are not working</t>
-  </si>
-  <si>
     <t>user password reset</t>
   </si>
   <si>
@@ -185,9 +173,6 @@
     <t>clause add</t>
   </si>
   <si>
-    <t>new clause form clauseref '000'</t>
-  </si>
-  <si>
     <t>action</t>
   </si>
   <si>
@@ -234,6 +219,18 @@
   </si>
   <si>
     <t>Add/delete clause</t>
+  </si>
+  <si>
+    <t>error on password does not fit in column</t>
+  </si>
+  <si>
+    <t>project edit and new errors are not working</t>
+  </si>
+  <si>
+    <t>no dot after prefix in jquery add</t>
+  </si>
+  <si>
+    <t>callback on loader gif not working properly - disable?</t>
   </si>
 </sst>
 </file>
@@ -584,8 +581,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -656,7 +653,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -667,7 +664,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -675,7 +672,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -683,43 +680,43 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
         <v>20</v>
       </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
         <v>22</v>
       </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
         <v>24</v>
       </c>
-      <c r="D15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>9</v>
       </c>
       <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
         <v>26</v>
-      </c>
-      <c r="D16" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -727,10 +724,10 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
         <v>28</v>
-      </c>
-      <c r="D17" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -738,158 +735,146 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
         <v>30</v>
       </c>
-      <c r="D18" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>9</v>
       </c>
-      <c r="C25" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" t="s">
-        <v>47</v>
-      </c>
-      <c r="D27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>51</v>
-      </c>
       <c r="D28" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="D31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>51</v>
-      </c>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>4</v>
-      </c>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D33">
+  <autoFilter ref="A1:D32">
     <filterColumn colId="0">
-      <filters>
-        <filter val="A"/>
-      </filters>
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -902,7 +887,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,18 +917,18 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -951,7 +936,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -959,7 +944,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -967,10 +952,10 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1015,7 +1000,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,15 +1008,15 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1039,7 +1024,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1054,7 +1039,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C18" sqref="C18:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1084,7 +1069,7 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1092,7 +1077,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1100,7 +1085,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1108,7 +1093,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1122,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="B7:C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,17 +1118,17 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
responsive design update 1
</commit_message>
<xml_diff>
--- a/code_managment.xlsx
+++ b/code_managment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="20955" windowHeight="9975"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="20955" windowHeight="9975" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Website" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
   <si>
     <t>location</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>callback on loader gif not working properly - disable?</t>
+  </si>
+  <si>
+    <t>bmp for prawn not working</t>
+  </si>
+  <si>
+    <t>admin user account alter</t>
   </si>
 </sst>
 </file>
@@ -573,10 +579,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,6 +851,14 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -865,7 +879,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,10 +959,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,10 +1013,18 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>